<commit_message>
update supp learning links
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule.xlsx
+++ b/docs/nopublish/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB2A1A7-E8B8-4E0E-9D81-B563F7C9088D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DE2914-D4EC-46E6-A63A-8F8A180BE47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2325" yWindow="2325" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11250" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="248">
   <si>
     <t>Week</t>
   </si>
@@ -762,6 +762,21 @@
   </si>
   <si>
     <t>[lectre10]</t>
+  </si>
+  <si>
+    <t>https://uoregon.zoom.us/rec/share/qucOfxWXjvjE1fn8itYTNI0iuUu2VucfyI_Itwe2LkN_NXmtmmg3Vomiekj7p642.LTaspw3WhyaidUW_</t>
+  </si>
+  <si>
+    <t>sbDc6$c2</t>
+  </si>
+  <si>
+    <t>https://www.codecademy.com/courses/learn-r/lessons/introduction-to-r/exercises/why-r</t>
+  </si>
+  <si>
+    <t>https://www.codecademy.com/courses/learn-r/lessons/intro-visualization-ggplot2-r/exercises/layers-and-geoms</t>
+  </si>
+  <si>
+    <t>https://www.codecademy.com/courses/learn-r/lessons/r-aggregates/exercises/column-statistics</t>
   </si>
 </sst>
 </file>
@@ -771,7 +786,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm;@"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -937,6 +952,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF232333"/>
+      <name val="Lato"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="36">
@@ -1326,7 +1347,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1373,6 +1394,8 @@
     <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1731,9 +1754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R3" sqref="R3"/>
+      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1853,8 +1876,12 @@
       <c r="K2" t="s">
         <v>75</v>
       </c>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
+      <c r="L2" s="22" t="s">
+        <v>243</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>244</v>
+      </c>
       <c r="N2" t="s">
         <v>11</v>
       </c>
@@ -2951,9 +2978,10 @@
     <hyperlink ref="P4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
     <hyperlink ref="S6" r:id="rId4" location="section-a-quick-tour-of-r-studio" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="P7" r:id="rId5" xr:uid="{093D27B3-CEE9-47CA-B053-E07A545793E3}"/>
+    <hyperlink ref="L2" r:id="rId6" xr:uid="{ACAAF725-A087-4762-8268-0223F4169356}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
 
@@ -3861,8 +3889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F2:F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4171,7 +4199,7 @@
       <c r="D12" s="6">
         <v>44839</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="33" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="21" t="s">
@@ -4197,11 +4225,11 @@
       <c r="D13" s="6">
         <v>44839</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="33" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>18</v>
+        <v>245</v>
       </c>
       <c r="G13" t="s">
         <v>239</v>
@@ -4223,10 +4251,10 @@
       <c r="D14" s="6">
         <v>44846</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="22" t="s">
         <v>47</v>
       </c>
       <c r="G14" t="s">
@@ -4252,7 +4280,7 @@
       <c r="E15" t="s">
         <v>34</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="22" t="s">
         <v>48</v>
       </c>
       <c r="G15" t="s">
@@ -4275,11 +4303,11 @@
       <c r="D16" s="6">
         <v>44846</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="F16" t="s">
-        <v>49</v>
+      <c r="F16" s="22" t="s">
+        <v>246</v>
       </c>
       <c r="G16" t="s">
         <v>239</v>
@@ -4301,10 +4329,10 @@
       <c r="D17" s="6">
         <v>44853</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="22" t="s">
         <v>78</v>
       </c>
       <c r="G17" t="s">
@@ -4353,11 +4381,11 @@
       <c r="D19" s="6">
         <v>44853</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E19" s="33" t="s">
         <v>60</v>
       </c>
-      <c r="F19" t="s">
-        <v>80</v>
+      <c r="F19" s="22" t="s">
+        <v>247</v>
       </c>
       <c r="G19" t="s">
         <v>239</v>
@@ -4379,10 +4407,10 @@
       <c r="D20" s="6">
         <v>44860</v>
       </c>
-      <c r="E20" t="s">
+      <c r="E20" s="33" t="s">
         <v>98</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="22" t="s">
         <v>111</v>
       </c>
       <c r="G20" t="s">
@@ -4405,7 +4433,7 @@
       <c r="D21" s="6">
         <v>44860</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="33" t="s">
         <v>100</v>
       </c>
       <c r="F21" t="s">
@@ -4511,8 +4539,14 @@
   <hyperlinks>
     <hyperlink ref="F12" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
     <hyperlink ref="F13" r:id="rId2" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="F16" r:id="rId3" xr:uid="{6671F9FF-37B4-4C93-A697-7D56C53820F9}"/>
+    <hyperlink ref="F19" r:id="rId4" xr:uid="{C1367910-9DF9-423C-9F03-8ABC43BA3664}"/>
+    <hyperlink ref="F14" r:id="rId5" xr:uid="{28570200-1C90-45B3-A75B-49AD8E4E58FB}"/>
+    <hyperlink ref="F17" r:id="rId6" xr:uid="{9E97C6B5-98EA-4509-9249-10F6BCF9DF73}"/>
+    <hyperlink ref="F20" r:id="rId7" xr:uid="{B0389D25-A1BB-4048-89BB-C95F8FF325CF}"/>
+    <hyperlink ref="F15" r:id="rId8" xr:uid="{2E2A5E1B-CDDC-477F-AE18-E9CD4F1FBD07}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add hw1, w2 slides
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule.xlsx
+++ b/docs/nopublish/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DE2914-D4EC-46E6-A63A-8F8A180BE47C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9F168A-D3FF-4E55-9517-331B435D7EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11250" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="548" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="249">
   <si>
     <t>Week</t>
   </si>
@@ -777,6 +777,9 @@
   </si>
   <si>
     <t>https://www.codecademy.com/courses/learn-r/lessons/r-aggregates/exercises/column-statistics</t>
+  </si>
+  <si>
+    <t>hw1.Rmd</t>
   </si>
 </sst>
 </file>
@@ -1754,30 +1757,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M3" sqref="M3"/>
+      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" customWidth="1"/>
     <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="16.86328125" customWidth="1"/>
+    <col min="14" max="14" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.265625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="31.42578125" customWidth="1"/>
-    <col min="20" max="20" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="31.3984375" customWidth="1"/>
+    <col min="20" max="20" width="56.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="23" customFormat="1">
@@ -1842,7 +1845,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
+    <row r="2" spans="1:20" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1938,7 +1941,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="8" customFormat="1" ht="15.75" thickBot="1">
+    <row r="5" spans="1:20" s="8" customFormat="1" ht="14.65" thickBot="1">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2100,7 +2103,9 @@
       <c r="N9" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="P9" s="26"/>
+      <c r="P9" s="26" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="10" spans="1:20" s="3" customFormat="1">
       <c r="A10" s="3">
@@ -2989,15 +2994,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C51" sqref="C51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3700,9 +3705,12 @@
       <c r="B51" s="4" t="s">
         <v>90</v>
       </c>
+      <c r="C51" t="s">
+        <v>248</v>
+      </c>
       <c r="D51" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[hw1]: </v>
+        <v>[hw1]: hw1.Rmd</v>
       </c>
     </row>
     <row r="52" spans="1:4">
@@ -3889,21 +3897,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.265625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.86328125" customWidth="1"/>
+    <col min="7" max="7" width="21.86328125" customWidth="1"/>
+    <col min="9" max="9" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3954,7 +3962,9 @@
       <c r="E2" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="27"/>
+      <c r="F2" s="33" t="s">
+        <v>248</v>
+      </c>
       <c r="H2">
         <v>10</v>
       </c>
@@ -4199,7 +4209,7 @@
       <c r="D12" s="6">
         <v>44839</v>
       </c>
-      <c r="E12" s="33" t="s">
+      <c r="E12" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="21" t="s">
@@ -4225,7 +4235,7 @@
       <c r="D13" s="6">
         <v>44839</v>
       </c>
-      <c r="E13" s="33" t="s">
+      <c r="E13" t="s">
         <v>14</v>
       </c>
       <c r="F13" s="21" t="s">
@@ -4251,7 +4261,7 @@
       <c r="D14" s="6">
         <v>44846</v>
       </c>
-      <c r="E14" s="33" t="s">
+      <c r="E14" t="s">
         <v>32</v>
       </c>
       <c r="F14" s="22" t="s">
@@ -4303,7 +4313,7 @@
       <c r="D16" s="6">
         <v>44846</v>
       </c>
-      <c r="E16" s="33" t="s">
+      <c r="E16" t="s">
         <v>36</v>
       </c>
       <c r="F16" s="22" t="s">
@@ -4329,7 +4339,7 @@
       <c r="D17" s="6">
         <v>44853</v>
       </c>
-      <c r="E17" s="33" t="s">
+      <c r="E17" t="s">
         <v>56</v>
       </c>
       <c r="F17" s="22" t="s">
@@ -4381,7 +4391,7 @@
       <c r="D19" s="6">
         <v>44853</v>
       </c>
-      <c r="E19" s="33" t="s">
+      <c r="E19" t="s">
         <v>60</v>
       </c>
       <c r="F19" s="22" t="s">
@@ -4407,7 +4417,7 @@
       <c r="D20" s="6">
         <v>44860</v>
       </c>
-      <c r="E20" s="33" t="s">
+      <c r="E20" t="s">
         <v>98</v>
       </c>
       <c r="F20" s="22" t="s">
@@ -4433,10 +4443,10 @@
       <c r="D21" s="6">
         <v>44860</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" t="s">
         <v>100</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="22" t="s">
         <v>112</v>
       </c>
       <c r="G21" t="s">
@@ -4545,8 +4555,9 @@
     <hyperlink ref="F17" r:id="rId6" xr:uid="{9E97C6B5-98EA-4509-9249-10F6BCF9DF73}"/>
     <hyperlink ref="F20" r:id="rId7" xr:uid="{B0389D25-A1BB-4048-89BB-C95F8FF325CF}"/>
     <hyperlink ref="F15" r:id="rId8" xr:uid="{2E2A5E1B-CDDC-477F-AE18-E9CD4F1FBD07}"/>
+    <hyperlink ref="F21" r:id="rId9" xr:uid="{FCBAD9A2-46E3-4C45-ADE7-DE1F58879DB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
w2 video and tweaks
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule.xlsx
+++ b/docs/nopublish/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9F168A-D3FF-4E55-9517-331B435D7EC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F791C52-CAC1-4735-86C3-6FB8049A66B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="551" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="251">
   <si>
     <t>Week</t>
   </si>
@@ -780,6 +780,12 @@
   </si>
   <si>
     <t>hw1.Rmd</t>
+  </si>
+  <si>
+    <t>https://uoregon.zoom.us/rec/share/NoSv0Jfaonj5XyktUE-q9QvWFwPrUApNv2Dh_Y7qJbmVirTvAFogOyHBf-axN1tW.Sx6xx4cHTEsXGAL_</t>
+  </si>
+  <si>
+    <t>n8%5MV$&amp;</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1356,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1398,7 +1404,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1759,7 +1766,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P9" sqref="P9"/>
+      <selection pane="bottomLeft" activeCell="M6" sqref="L6:M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -1845,7 +1852,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:20" ht="15">
+    <row r="2" spans="1:20">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1960,7 +1967,7 @@
       </c>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:20" s="2" customFormat="1">
+    <row r="6" spans="1:20" s="2" customFormat="1" ht="15">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -1994,7 +2001,12 @@
       <c r="K6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="20"/>
+      <c r="L6" s="33" t="s">
+        <v>249</v>
+      </c>
+      <c r="M6" s="34" t="s">
+        <v>250</v>
+      </c>
       <c r="N6" s="2" t="s">
         <v>32</v>
       </c>
@@ -2984,9 +2996,10 @@
     <hyperlink ref="S6" r:id="rId4" location="section-a-quick-tour-of-r-studio" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
     <hyperlink ref="P7" r:id="rId5" xr:uid="{093D27B3-CEE9-47CA-B053-E07A545793E3}"/>
     <hyperlink ref="L2" r:id="rId6" xr:uid="{ACAAF725-A087-4762-8268-0223F4169356}"/>
+    <hyperlink ref="L6" r:id="rId7" display="https://urldefense.com/v3/__https:/uoregon.zoom.us/rec/share/NoSv0Jfaonj5XyktUE-q9QvWFwPrUApNv2Dh_Y7qJbmVirTvAFogOyHBf-axN1tW.Sx6xx4cHTEsXGAL___;!!C5qS4YX3!DMidTfFsH9V66gHPZmGeZOXWm-TF2pCxxaXDUkGb6Z-iUoBMRwyOcP9WSjX6iTgw7OmnO89n47n3fgqexg$" xr:uid="{495C90F6-7392-419F-90AA-E59BC195E6A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -3898,7 +3911,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
@@ -3962,7 +3975,7 @@
       <c r="E2" t="s">
         <v>229</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" t="s">
         <v>248</v>
       </c>
       <c r="H2">

</xml_diff>

<commit_message>
add hws 2 and 3
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule.xlsx
+++ b/docs/nopublish/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F791C52-CAC1-4735-86C3-6FB8049A66B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3272829C-75D7-4C8A-A242-09C71B78A56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="253">
   <si>
     <t>Week</t>
   </si>
@@ -786,6 +786,12 @@
   </si>
   <si>
     <t>n8%5MV$&amp;</t>
+  </si>
+  <si>
+    <t>hw2-key.pdf</t>
+  </si>
+  <si>
+    <t>hw3.Rmd</t>
   </si>
 </sst>
 </file>
@@ -1400,12 +1406,10 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="35" borderId="0" xfId="42" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="42" applyFill="1"/>
     <xf numFmtId="0" fontId="23" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1764,30 +1768,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="N1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M6" sqref="L6:M6"/>
+      <selection pane="bottomLeft" activeCell="P14" sqref="P14:P15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.73046875" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.3984375" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" customWidth="1"/>
     <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.86328125" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.73046875" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="16.86328125" customWidth="1"/>
-    <col min="14" max="14" width="47.265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="16.85546875" customWidth="1"/>
+    <col min="14" max="14" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="36.86328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="31.3984375" customWidth="1"/>
-    <col min="20" max="20" width="56.73046875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="31.42578125" customWidth="1"/>
+    <col min="20" max="20" width="56.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="23" customFormat="1">
@@ -1889,7 +1893,7 @@
       <c r="L2" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="31" t="s">
         <v>244</v>
       </c>
       <c r="N2" t="s">
@@ -1948,7 +1952,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="8" customFormat="1" ht="14.65" thickBot="1">
+    <row r="5" spans="1:20" s="8" customFormat="1" ht="15.75" thickBot="1">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -1967,7 +1971,7 @@
       </c>
       <c r="O5" s="10"/>
     </row>
-    <row r="6" spans="1:20" s="2" customFormat="1" ht="15">
+    <row r="6" spans="1:20" s="2" customFormat="1">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -2001,10 +2005,10 @@
       <c r="K6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="L6" s="33" t="s">
+      <c r="L6" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="M6" s="34" t="s">
+      <c r="M6" s="33" t="s">
         <v>250</v>
       </c>
       <c r="N6" s="2" t="s">
@@ -2271,14 +2275,18 @@
       <c r="O14" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="P14" s="27"/>
+      <c r="P14" s="27" t="s">
+        <v>251</v>
+      </c>
       <c r="Q14" t="s">
         <v>229</v>
       </c>
       <c r="R14" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="S14" s="26"/>
+      <c r="S14" s="26" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="15" spans="1:20" s="8" customFormat="1">
       <c r="A15" s="8">
@@ -2291,7 +2299,9 @@
       <c r="O15" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="P15" s="28"/>
+      <c r="P15" s="28" t="s">
+        <v>252</v>
+      </c>
       <c r="Q15" s="8" t="s">
         <v>61</v>
       </c>
@@ -2426,7 +2436,9 @@
       <c r="R19" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="S19" s="26"/>
+      <c r="S19" s="27" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="20" spans="1:20" s="3" customFormat="1">
       <c r="A20" s="3">
@@ -2439,7 +2451,9 @@
       <c r="R20" s="18" t="s">
         <v>95</v>
       </c>
-      <c r="S20" s="31"/>
+      <c r="S20" s="28" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="21" spans="1:20">
       <c r="A21" s="11">
@@ -3007,15 +3021,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53:C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3745,9 +3759,12 @@
       <c r="B53" s="4" t="s">
         <v>94</v>
       </c>
+      <c r="C53" s="34" t="s">
+        <v>251</v>
+      </c>
       <c r="D53" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[hw2]: </v>
+        <v>[hw2]: hw2-key.pdf</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -3757,9 +3774,12 @@
       <c r="B54" s="4" t="s">
         <v>95</v>
       </c>
+      <c r="C54" s="34" t="s">
+        <v>252</v>
+      </c>
       <c r="D54" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">[hw3]: </v>
+        <v>[hw3]: hw3.Rmd</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -3910,21 +3930,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.265625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.265625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="47.265625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.86328125" customWidth="1"/>
-    <col min="7" max="7" width="21.86328125" customWidth="1"/>
-    <col min="9" max="9" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4002,7 +4022,9 @@
       <c r="E3" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="34" t="s">
+        <v>251</v>
+      </c>
       <c r="H3">
         <v>10</v>
       </c>
@@ -4027,7 +4049,9 @@
       <c r="E4" t="s">
         <v>222</v>
       </c>
-      <c r="F4" s="27"/>
+      <c r="F4" s="34" t="s">
+        <v>252</v>
+      </c>
       <c r="H4">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
add HW1 key & w3 zoom
</commit_message>
<xml_diff>
--- a/docs/nopublish/schedule.xlsx
+++ b/docs/nopublish/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jnese\Desktop\BRT\Teaching\1_Intro-Data-Science\c1-intro-fall-2022\nopublish\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3272829C-75D7-4C8A-A242-09C71B78A56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1268EC-A2D3-4521-A30C-9545495D0B90}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="schedule" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="562" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="256">
   <si>
     <t>Week</t>
   </si>
@@ -792,6 +792,15 @@
   </si>
   <si>
     <t>hw3.Rmd</t>
+  </si>
+  <si>
+    <t>hw1-key.html</t>
+  </si>
+  <si>
+    <t>https://uoregon.zoom.us/rec/share/vAVpHmKukubq75B5MlOqhnfiTaCZsH2x1-HkXaUv83XT0elfVSj205NXDRk0EAnD.4SIowxSyQJCWj9bh</t>
+  </si>
+  <si>
+    <t>%V*z$W2n</t>
   </si>
 </sst>
 </file>
@@ -1768,30 +1777,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X42"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P14" sqref="P14:P15"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.73046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.86328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.3984375" customWidth="1"/>
     <col min="6" max="6" width="59" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.86328125" customWidth="1"/>
     <col min="9" max="9" width="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="26.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="16.85546875" customWidth="1"/>
-    <col min="14" max="14" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="16.86328125" customWidth="1"/>
+    <col min="14" max="14" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.265625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="20" customWidth="1"/>
-    <col min="17" max="17" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="31.42578125" customWidth="1"/>
-    <col min="20" max="20" width="56.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.86328125" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="31.3984375" customWidth="1"/>
+    <col min="20" max="20" width="56.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" s="23" customFormat="1">
@@ -1952,7 +1961,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:20" s="8" customFormat="1" ht="15.75" thickBot="1">
+    <row r="5" spans="1:20" s="8" customFormat="1" ht="14.65" thickBot="1">
       <c r="A5" s="8">
         <v>1</v>
       </c>
@@ -2172,7 +2181,12 @@
       <c r="K11" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="L11" s="22"/>
+      <c r="L11" s="22" t="s">
+        <v>254</v>
+      </c>
+      <c r="M11" s="34" t="s">
+        <v>255</v>
+      </c>
       <c r="N11" s="11" t="s">
         <v>56</v>
       </c>
@@ -3011,9 +3025,10 @@
     <hyperlink ref="P7" r:id="rId5" xr:uid="{093D27B3-CEE9-47CA-B053-E07A545793E3}"/>
     <hyperlink ref="L2" r:id="rId6" xr:uid="{ACAAF725-A087-4762-8268-0223F4169356}"/>
     <hyperlink ref="L6" r:id="rId7" display="https://urldefense.com/v3/__https:/uoregon.zoom.us/rec/share/NoSv0Jfaonj5XyktUE-q9QvWFwPrUApNv2Dh_Y7qJbmVirTvAFogOyHBf-axN1tW.Sx6xx4cHTEsXGAL___;!!C5qS4YX3!DMidTfFsH9V66gHPZmGeZOXWm-TF2pCxxaXDUkGb6Z-iUoBMRwyOcP9WSjX6iTgw7OmnO89n47n3fgqexg$" xr:uid="{495C90F6-7392-419F-90AA-E59BC195E6A3}"/>
+    <hyperlink ref="L11" r:id="rId8" xr:uid="{430F5ABF-D6F3-4170-B9C7-CB0C5D200272}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId8"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
@@ -3021,15 +3036,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A32" workbookViewId="0">
       <selection activeCell="C53" sqref="C53:C54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="100.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="100.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -3759,7 +3774,7 @@
       <c r="B53" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="C53" s="34" t="s">
+      <c r="C53" t="s">
         <v>251</v>
       </c>
       <c r="D53" t="str">
@@ -3774,7 +3789,7 @@
       <c r="B54" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="C54" s="34" t="s">
+      <c r="C54" t="s">
         <v>252</v>
       </c>
       <c r="D54" t="str">
@@ -3930,21 +3945,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:J26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="47.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.85546875" customWidth="1"/>
-    <col min="7" max="7" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.265625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.265625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="47.265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.86328125" customWidth="1"/>
+    <col min="7" max="7" width="21.86328125" customWidth="1"/>
+    <col min="9" max="9" width="10.86328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="27.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -4004,7 +4019,9 @@
       <c r="I2" t="s">
         <v>230</v>
       </c>
-      <c r="J2" s="27"/>
+      <c r="J2" t="s">
+        <v>253</v>
+      </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3">
@@ -4022,7 +4039,7 @@
       <c r="E3" t="s">
         <v>221</v>
       </c>
-      <c r="F3" s="34" t="s">
+      <c r="F3" t="s">
         <v>251</v>
       </c>
       <c r="H3">
@@ -4049,7 +4066,7 @@
       <c r="E4" t="s">
         <v>222</v>
       </c>
-      <c r="F4" s="34" t="s">
+      <c r="F4" t="s">
         <v>252</v>
       </c>
       <c r="H4">

</xml_diff>